<commit_message>
Basic code - first assessment completed
</commit_message>
<xml_diff>
--- a/Selenium/Data/Data for BootCamp.xlsx
+++ b/Selenium/Data/Data for BootCamp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/palanimohan/git/Local Repository/Selenium/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C5C527-FF71-2246-954E-76143E7E290C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC40B7C-BAB9-5547-A386-762D77D0147B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16640" xr2:uid="{51DA2A99-B2E2-BB47-A8CA-640766803AEA}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16640" activeTab="1" xr2:uid="{51DA2A99-B2E2-BB47-A8CA-640766803AEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Board Exam Schedule" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="16">
   <si>
     <t>User Name</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>JKL</t>
-  </si>
-  <si>
-    <t>MNO</t>
   </si>
   <si>
     <t>PQR</t>
@@ -99,7 +96,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -109,6 +106,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -131,14 +136,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -453,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7440F90E-3A50-E34E-8F91-993B610BB968}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -466,7 +474,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -480,7 +488,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -494,10 +502,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
@@ -514,10 +522,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF68CA1E-3746-2C4E-904B-1109E10B84AF}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -529,7 +537,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -543,7 +551,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -552,20 +560,6 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -579,7 +573,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -591,7 +585,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -605,24 +599,24 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
@@ -632,6 +626,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{02F5285E-3995-254D-86ED-A3E76620940F}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{8733217E-9873-9E45-B4B5-8CC25E259847}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{D7536289-FE51-4443-9D56-8FC2D8D7A427}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -653,7 +652,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -667,7 +666,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -681,7 +680,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
@@ -715,7 +714,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -729,7 +728,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -743,7 +742,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
@@ -777,7 +776,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -791,7 +790,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -805,7 +804,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -839,7 +838,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -853,7 +852,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -867,7 +866,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -901,7 +900,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -915,7 +914,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -929,7 +928,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -963,7 +962,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -977,7 +976,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -991,7 +990,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
POM Project and Other Changes
</commit_message>
<xml_diff>
--- a/Selenium/Data/Data for BootCamp.xlsx
+++ b/Selenium/Data/Data for BootCamp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/palanimohan/git/Local Repository/Selenium/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC40B7C-BAB9-5547-A386-762D77D0147B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534ABB9A-7429-8244-8F55-E366EBD183BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16640" activeTab="1" xr2:uid="{51DA2A99-B2E2-BB47-A8CA-640766803AEA}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16640" activeTab="7" xr2:uid="{51DA2A99-B2E2-BB47-A8CA-640766803AEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Board Exam Schedule" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="26">
   <si>
     <t>User Name</t>
   </si>
@@ -62,34 +62,64 @@
     <t>cypress@testleaf.com</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Best</t>
-  </si>
-  <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>DEF</t>
-  </si>
-  <si>
-    <t>GHI</t>
-  </si>
-  <si>
-    <t>JKL</t>
-  </si>
-  <si>
-    <t>PQR</t>
-  </si>
-  <si>
     <t>Browser</t>
   </si>
   <si>
     <t>Chrome</t>
   </si>
   <si>
-    <t>Firefox</t>
+    <t>Goal</t>
+  </si>
+  <si>
+    <t>Dashboard Name</t>
+  </si>
+  <si>
+    <t>Dashboard Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palanimohan_Workout </t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>10:00 AM</t>
+  </si>
+  <si>
+    <t>Opportunity Name</t>
+  </si>
+  <si>
+    <t>Salesforce Automation by Palanimohan</t>
+  </si>
+  <si>
+    <t>Task Name</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Sarath M</t>
+  </si>
+  <si>
+    <t>Boot Camp</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>SALES FORCE Automation Using Selenium</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Chart Name</t>
+  </si>
+  <si>
+    <t>Practice Chart</t>
   </si>
 </sst>
 </file>
@@ -140,10 +170,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -459,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7440F90E-3A50-E34E-8F91-993B610BB968}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -474,7 +506,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -488,7 +520,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -497,20 +529,6 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -522,10 +540,149 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF68CA1E-3746-2C4E-904B-1109E10B84AF}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>10000</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{6B34EEF3-FCAC-B047-BCD8-38AFD416C7BC}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{42FF37F3-0BAA-324C-B3E7-9968831266AE}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{0865407F-AEF9-E84A-994B-3F754DE048F4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D7D221F-0419-1D47-8B77-B31F9B7BE733}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{02F5285E-3995-254D-86ED-A3E76620940F}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{8733217E-9873-9E45-B4B5-8CC25E259847}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{D7536289-FE51-4443-9D56-8FC2D8D7A427}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587C070B-0B85-0F43-B9A3-659F364D9359}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -535,9 +692,9 @@
     <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -548,10 +705,16 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -561,6 +724,12 @@
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -568,9 +737,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D7D221F-0419-1D47-8B77-B31F9B7BE733}">
-  <dimension ref="A1:D3"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6498A40E-F5B8-504D-8FA8-538281D0422D}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
@@ -585,7 +754,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -599,48 +768,29 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{02F5285E-3995-254D-86ED-A3E76620940F}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{8733217E-9873-9E45-B4B5-8CC25E259847}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{D7536289-FE51-4443-9D56-8FC2D8D7A427}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587C070B-0B85-0F43-B9A3-659F364D9359}">
-  <dimension ref="A1:D3"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC2A2433-10CD-6B4A-BDDC-9A0911EC4086}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -652,7 +802,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -666,7 +816,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -675,20 +825,6 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -697,12 +833,73 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6498A40E-F5B8-504D-8FA8-538281D0422D}">
-  <dimension ref="A1:D3"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{730641D4-73FA-2543-9F29-DFF47F21C48A}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FCDBAA1-8A61-3644-930F-DE52A1B68E9E}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -712,9 +909,9 @@
     <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -725,10 +922,13 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -739,19 +939,8 @@
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
+      <c r="E2" s="4">
+        <v>5000</v>
       </c>
     </row>
   </sheetData>
@@ -759,12 +948,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC2A2433-10CD-6B4A-BDDC-9A0911EC4086}">
-  <dimension ref="A1:D3"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44CE971E-3B72-044E-8D82-556BCA63A96D}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -774,9 +963,9 @@
     <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -787,10 +976,13 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -801,205 +993,8 @@
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{730641D4-73FA-2543-9F29-DFF47F21C48A}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FCDBAA1-8A61-3644-930F-DE52A1B68E9E}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44CE971E-3B72-044E-8D82-556BCA63A96D}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
+      <c r="E2" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>